<commit_message>
Changed .zip files from openthread
</commit_message>
<xml_diff>
--- a/Benchmark Management/Config.xlsx
+++ b/Benchmark Management/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raffael\GitHub\P6_Software\Benchmark Managment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\GitHub\P6_Software\Benchmark Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18000064-E81E-4CB7-B806-B62EB477774F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7753CB-7631-47DA-B132-DB5EB4BC749F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
   <si>
     <t>Number</t>
   </si>
@@ -304,8 +304,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:E9" totalsRowShown="0">
-  <autoFilter ref="A1:E9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Firmware"/>
@@ -616,7 +616,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,147 +647,94 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>7928FDBD</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2</v>
-      </c>
+        <v>16D87965</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>E1A6E5BF</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
+        <v>228D1458</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>DC94CD5B</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
+        <v>B6D10C96</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>A4F21E13</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3</v>
-      </c>
+        <v>E5B83E8E</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>EA97A00B</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
+        <v>52993E8A</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>70AAAF03</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
+        <v>8E323CE7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="str">
         <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>5BEB2713</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
+        <v>6776E907</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" t="str">
-        <f>VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE)</f>
-        <v>E22399C0</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
+      <c r="E9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -801,19 +748,19 @@
           <x14:formula1>
             <xm:f>Constants!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B9</xm:sqref>
+          <xm:sqref>B2:B8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BED282B8-5A63-432E-8F33-CB3377B63A1C}">
           <x14:formula1>
             <xm:f>Constants!$F$2:$F$27</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:E9</xm:sqref>
+          <xm:sqref>D2:E8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE6EC81D-B64F-49DB-9E36-AE4995FCB78F}">
           <x14:formula1>
             <xm:f>Constants!$C$2:$C$54</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A9</xm:sqref>
+          <xm:sqref>A2:A8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Benchmark Management for Zigbee
</commit_message>
<xml_diff>
--- a/Benchmark Management/Config.xlsx
+++ b/Benchmark Management/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril\Documents\GitHub\P6_Software\Benchmark Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9CF89C-D8C8-4B21-9707-C526CEE74678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22A3F5E-67AA-46E0-8080-07ACD42B2CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Number</t>
   </si>
@@ -346,8 +346,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:M3" totalsRowShown="0">
-  <autoFilter ref="A1:M3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:M7" totalsRowShown="0">
+  <autoFilter ref="A1:M7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Firmware"/>
@@ -669,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,37 +734,40 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C2" t="str">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</f>
-        <v>13D67795</v>
+        <v>7928FDBD</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>120</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
       </c>
       <c r="I2" t="str">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
-        <v>7928FDBD</v>
-      </c>
-      <c r="K2">
+        <v>E1A6E5BF</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2" t="str">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
-        <v>0</v>
+        <v>A7A6C5A8</v>
       </c>
       <c r="M2">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
@@ -773,39 +776,186 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C3" t="str">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</f>
-        <v>F5EA067B</v>
+        <v>E1A6E5BF</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="str">
+      <c r="I3">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
-        <v>7928FDBD</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="M3">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</f>
+        <v>A7A6C5A8</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4" t="str">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</f>
+        <v>8E323CE7</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5" s="4" t="str">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
+        <v>7C92D6F4</v>
+      </c>
+      <c r="K5" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</f>
+        <v>7C92D6F4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="str">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</f>
+        <v>DC94CD5B</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
+        <v>A7A6C5A8</v>
+      </c>
+      <c r="K7" s="4">
+        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
         <v>0</v>
       </c>
@@ -823,19 +973,19 @@
           <x14:formula1>
             <xm:f>Constants!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
+          <xm:sqref>B2:B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BED282B8-5A63-432E-8F33-CB3377B63A1C}">
           <x14:formula1>
             <xm:f>Constants!$F$2:$F$27</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:E3</xm:sqref>
+          <xm:sqref>D2:E7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE6EC81D-B64F-49DB-9E36-AE4995FCB78F}">
           <x14:formula1>
             <xm:f>Constants!$C$2:$C$54</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A3 H2:H3 J2:J3 L2:L3</xm:sqref>
+          <xm:sqref>A2:A7 H2:H7 J2:J7 L2:L7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -847,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Zigbee no groups debug finished
</commit_message>
<xml_diff>
--- a/Benchmark Management/Config.xlsx
+++ b/Benchmark Management/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril\Documents\GitHub\P6_Software\Benchmark Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22A3F5E-67AA-46E0-8080-07ACD42B2CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4243F74D-3910-465E-A090-1EE60D6272E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>Number</t>
   </si>
@@ -346,8 +346,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:M7" totalsRowShown="0">
-  <autoFilter ref="A1:M7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:M5" totalsRowShown="0">
+  <autoFilter ref="A1:M5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Firmware"/>
@@ -669,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,10 +744,10 @@
         <v>7928FDBD</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -762,12 +762,9 @@
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
         <v>E1A6E5BF</v>
       </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2" t="str">
+      <c r="K2">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
-        <v>A7A6C5A8</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
@@ -786,10 +783,10 @@
         <v>E1A6E5BF</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -822,10 +819,10 @@
         <v>A7A6C5A8</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -858,10 +855,10 @@
         <v>8E323CE7</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -870,92 +867,17 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I5" s="4" t="str">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
-        <v>7C92D6F4</v>
+        <v>A7A6C5A8</v>
       </c>
       <c r="K5" s="4">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="M5" s="4">
-        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</f>
-        <v>7C92D6F4</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="4" t="str">
-        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</f>
-        <v>DC94CD5B</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7" s="4" t="str">
-        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</f>
-        <v>A7A6C5A8</v>
-      </c>
-      <c r="K7" s="4">
-        <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_2]],Tabelle3[],2,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
         <f>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_3]],Tabelle3[],2,FALSE),0)</f>
         <v>0</v>
       </c>
@@ -973,19 +895,19 @@
           <x14:formula1>
             <xm:f>Constants!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B7</xm:sqref>
+          <xm:sqref>B2:B5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BED282B8-5A63-432E-8F33-CB3377B63A1C}">
           <x14:formula1>
             <xm:f>Constants!$F$2:$F$27</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:E7</xm:sqref>
+          <xm:sqref>D2:E5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE6EC81D-B64F-49DB-9E36-AE4995FCB78F}">
           <x14:formula1>
             <xm:f>Constants!$C$2:$C$54</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A7 H2:H7 J2:J7 L2:L7</xm:sqref>
+          <xm:sqref>A2:A5 H2:H5 J2:J5 L2:L5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added Active Radio Time
</commit_message>
<xml_diff>
--- a/Benchmark Management/Config.xlsx
+++ b/Benchmark Management/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raffael\GitHub\P6_Software\Benchmark Managment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raffael\GitHub\P6_Software\Benchmark Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E849DE83-9A81-441F-8807-7733F306BB2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1593490D-B8C1-4203-8DFD-7C0ECFF0B71F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,7 +312,10 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -324,10 +327,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -351,15 +351,15 @@
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Number"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Firmware"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Dev ID" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Dev ID" dataDxfId="6">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabelle1[[#This Row],[Number]],Tabelle3[],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Group ID"/>
-    <tableColumn id="5" xr3:uid="{BF33E156-0868-4FE7-AEB6-BAA4A1A6CAB8}" name="Node Id" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{BF33E156-0868-4FE7-AEB6-BAA4A1A6CAB8}" name="Node Id" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{00047FA1-B776-4161-9A5E-61CD291BFDE7}" name="Ack"/>
     <tableColumn id="7" xr3:uid="{1127329E-899C-4626-93A4-7D09EBA3B157}" name="Add Payload Len"/>
     <tableColumn id="8" xr3:uid="{FCC38A83-0D45-4F8E-B2DD-7BAAAA942F45}" name="DST_Node_1"/>
-    <tableColumn id="12" xr3:uid="{87E21627-A692-445A-A2CA-36DDBC7DA312}" name="DST_MAC_1" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{87E21627-A692-445A-A2CA-36DDBC7DA312}" name="DST_MAC_1" dataDxfId="4">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Tabelle1[[#This Row],[DST_Node_1]],Tabelle3[],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{2A65C8C5-CF0D-4044-9EF1-81065B5FA9F5}" name="DST_Node_2"/>
@@ -389,8 +389,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle3" displayName="Tabelle3" ref="C1:D54" totalsRowShown="0">
   <autoFilter ref="C1:D54" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Number" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Device ID" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Number" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Device ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -672,7 +672,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D21:D22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added ot_master for PCA10056 in config.xlsx
</commit_message>
<xml_diff>
--- a/Benchmark Management/Config.xlsx
+++ b/Benchmark Management/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\GitHub\P6_Software\Benchmark Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438E83AD-CD0B-4A73-B5D2-9453AB6DF1A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351BAB40-2360-4C4D-A6E8-AC3F678CCAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2540,12 +2540,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2A9CFBD8-98C6-47B7-83CE-7D8A4658D465}">
           <x14:formula1>
             <xm:f>Constants!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B51</xm:sqref>
+          <xm:sqref>B3:B51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BED282B8-5A63-432E-8F33-CB3377B63A1C}">
           <x14:formula1>
@@ -2559,6 +2559,12 @@
           </x14:formula1>
           <xm:sqref>A2:A51 L2:L51 J2:J51 H2:H51</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D65AA8E7-A56D-4716-9F74-FB4AD27C34AB}">
+          <x14:formula1>
+            <xm:f>Constants!$A$2:$A$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2569,7 +2575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>